<commit_message>
added initial version of machine learning
</commit_message>
<xml_diff>
--- a/sample/CatwalkHeaders.xlsx
+++ b/sample/CatwalkHeaders.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nsg/PycharmProjects/CAT/sample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B36804-01F9-C54C-9D76-4C6CEC02F800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0290AB11-4518-BA49-8A55-6E330D88CEC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="400">
   <si>
     <t>Experiment</t>
   </si>
@@ -1171,6 +1171,69 @@
   </si>
   <si>
     <t>Support_Four_(%)</t>
+  </si>
+  <si>
+    <t>BodySpeed_(mm/s)_Mean</t>
+  </si>
+  <si>
+    <t>Stand_(s)_Mean</t>
+  </si>
+  <si>
+    <t>MaxContactAt_(%)_Mean</t>
+  </si>
+  <si>
+    <t>MaxContactArea_(mm²)_Mean</t>
+  </si>
+  <si>
+    <t>StandIndex_Mean</t>
+  </si>
+  <si>
+    <t>MaxContactMaxIntensity_Mean</t>
+  </si>
+  <si>
+    <t>MaxContactMeanIntensity_Mean</t>
+  </si>
+  <si>
+    <t>PrintLength_(mm)_Mean</t>
+  </si>
+  <si>
+    <t>PrintWidth_(mm)_Mean</t>
+  </si>
+  <si>
+    <t>PrintArea_(mm²)_Mean</t>
+  </si>
+  <si>
+    <t>MaxIntensityAt_(%)_Mean</t>
+  </si>
+  <si>
+    <t>MaxIntensity_Mean</t>
+  </si>
+  <si>
+    <t>MeanIntensity_Mean</t>
+  </si>
+  <si>
+    <t>Swing_(s)_Mean</t>
+  </si>
+  <si>
+    <t>SwingSpeed_(mm/s)_Mean</t>
+  </si>
+  <si>
+    <t>StrideLength_(mm)_Mean</t>
+  </si>
+  <si>
+    <t>StepCycle_(s)_Mean</t>
+  </si>
+  <si>
+    <t>BodySpeedVariation_(%)_Mean</t>
+  </si>
+  <si>
+    <t>SingleStance_(s)_Mean</t>
+  </si>
+  <si>
+    <t>InitialDualStance_(s)_Mean</t>
+  </si>
+  <si>
+    <t>TerminalDualStance_(s)_Mean</t>
   </si>
 </sst>
 </file>
@@ -1494,17 +1557,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B379"/>
+  <dimension ref="A1:S379"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <pane ySplit="6140" topLeftCell="A251"/>
-      <selection activeCell="B10" sqref="B1:B10"/>
-      <selection pane="bottomLeft" activeCell="A257" sqref="A257:B258"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="6140" topLeftCell="A425"/>
+      <selection activeCell="S81" sqref="S81:S83"/>
+      <selection pane="bottomLeft" activeCell="A243" sqref="A243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="49.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -2082,7 +2146,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>64</v>
       </c>
@@ -2091,7 +2155,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>65</v>
       </c>
@@ -2100,7 +2164,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>66</v>
       </c>
@@ -2109,7 +2173,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>67</v>
       </c>
@@ -2118,7 +2182,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>68</v>
       </c>
@@ -2127,7 +2191,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>69</v>
       </c>
@@ -2136,7 +2200,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>70</v>
       </c>
@@ -2145,7 +2209,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>71</v>
       </c>
@@ -2154,7 +2218,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>72</v>
       </c>
@@ -2162,8 +2226,20 @@
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H73" t="s">
+        <v>386</v>
+      </c>
+      <c r="L73" t="s">
+        <v>380</v>
+      </c>
+      <c r="N73" t="s">
+        <v>379</v>
+      </c>
+      <c r="S73" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>73</v>
       </c>
@@ -2171,8 +2247,20 @@
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H74" t="s">
+        <v>387</v>
+      </c>
+      <c r="L74" t="s">
+        <v>383</v>
+      </c>
+      <c r="N74" t="s">
+        <v>396</v>
+      </c>
+      <c r="S74" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>74</v>
       </c>
@@ -2180,8 +2268,14 @@
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H75" t="s">
+        <v>388</v>
+      </c>
+      <c r="S75" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>75</v>
       </c>
@@ -2189,8 +2283,11 @@
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="S76" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>76</v>
       </c>
@@ -2199,7 +2296,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>77</v>
       </c>
@@ -2208,7 +2305,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>78</v>
       </c>
@@ -2217,7 +2314,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>79</v>
       </c>
@@ -2226,7 +2323,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>80</v>
       </c>
@@ -2234,8 +2331,11 @@
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="S81" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>81</v>
       </c>
@@ -2243,8 +2343,11 @@
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="S82" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>82</v>
       </c>
@@ -2252,8 +2355,11 @@
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="S83" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>83</v>
       </c>
@@ -2261,8 +2367,14 @@
         <f t="shared" si="1"/>
         <v>83</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H84" t="s">
+        <v>392</v>
+      </c>
+      <c r="L84" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>84</v>
       </c>
@@ -2270,8 +2382,14 @@
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H85" t="s">
+        <v>393</v>
+      </c>
+      <c r="L85" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>85</v>
       </c>
@@ -2279,8 +2397,14 @@
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H86" t="s">
+        <v>394</v>
+      </c>
+      <c r="L86" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>86</v>
       </c>
@@ -2288,8 +2412,11 @@
         <f t="shared" si="1"/>
         <v>86</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="H87" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>87</v>
       </c>
@@ -2298,7 +2425,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>88</v>
       </c>
@@ -2307,7 +2434,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>89</v>
       </c>
@@ -2316,7 +2443,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>90</v>
       </c>
@@ -2325,7 +2452,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>91</v>
       </c>
@@ -2334,7 +2461,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>92</v>
       </c>
@@ -2343,7 +2470,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>93</v>
       </c>
@@ -2352,7 +2479,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>94</v>
       </c>
@@ -2361,7 +2488,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>95</v>
       </c>
@@ -4919,5 +5046,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>